<commit_message>
adding level 2 map
</commit_message>
<xml_diff>
--- a/level3_class.xlsx
+++ b/level3_class.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17000" yWindow="0" windowWidth="10900" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="17000" yWindow="0" windowWidth="10900" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="3" sheetId="1" r:id="rId1"/>
+    <sheet name="2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="33">
   <si>
     <t>Number</t>
   </si>
@@ -91,16 +92,59 @@
   </si>
   <si>
     <t>circulatory &amp;cardiac system</t>
+  </si>
+  <si>
+    <t>Studio</t>
+  </si>
+  <si>
+    <t>bug box</t>
+  </si>
+  <si>
+    <t>puzzle area</t>
+  </si>
+  <si>
+    <t>interactive game</t>
+  </si>
+  <si>
+    <t>spinning section</t>
+  </si>
+  <si>
+    <t>disco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power </t>
+  </si>
+  <si>
+    <t>planes</t>
+  </si>
+  <si>
+    <t>poster exhibit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,13 +167,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -812,6 +860,230 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>